<commit_message>
Beginning of Lesson and teacher management feature
</commit_message>
<xml_diff>
--- a/assets/sheets/profildapodik.xlsx
+++ b/assets/sheets/profildapodik.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Profil SD ISLAM AL KHAIRIYA" sheetId="1" state="visible" r:id="rId2"/>
@@ -4061,8 +4061,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D54" activeCellId="0" sqref="D54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5278,7 +5278,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="20" min="18" style="0" width="13.02"/>
@@ -15363,10 +15363,10 @@
   </sheetPr>
   <dimension ref="A1:J199"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J204" activeCellId="0" sqref="J204"/>
+      <selection pane="bottomLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>